<commit_message>
Cập nhật file mẫu excel hiệu suất nhân viên, kpi nhóm khác
Ràng buộc thêm các điều kiện khi tạo kpi nhóm khác.
</commit_message>
<xml_diff>
--- a/kpi/WebContent/resources/maufile/kpinhanvien.xlsx
+++ b/kpi/WebContent/resources/maufile/kpinhanvien.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lixco\Desktop\Image Chuong Trinh KPI\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lixco\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="2370" windowHeight="0"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="27405" windowHeight="12915"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>MÃ VỊ TRÍ</t>
   </si>
@@ -54,6 +54,9 @@
   </si>
   <si>
     <t>Đảm bảo gửi báo cáo phân tích tình hình biến động nhân sự qua chỉ số nghỉ việc hàng tháng trước ngày 5 hàng tháng.</t>
+  </si>
+  <si>
+    <t>ĐIỂM TRỪ (%)</t>
   </si>
 </sst>
 </file>
@@ -415,20 +418,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="58.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20" style="1" customWidth="1"/>
+    <col min="3" max="4" width="20" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -438,8 +441,11 @@
       <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D1" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>3002104</v>
       </c>
@@ -449,8 +455,9 @@
       <c r="C2" s="5">
         <v>24</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="D2" s="5"/>
+    </row>
+    <row r="3" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>3002104</v>
       </c>
@@ -460,8 +467,11 @@
       <c r="C3" s="5">
         <v>29</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="D3" s="5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>3002104</v>
       </c>
@@ -471,8 +481,9 @@
       <c r="C4" s="5">
         <v>29</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="D4" s="5"/>
+    </row>
+    <row r="5" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>3002105</v>
       </c>
@@ -482,8 +493,9 @@
       <c r="C5" s="5">
         <v>29</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="D5" s="5"/>
+    </row>
+    <row r="6" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>3002105</v>
       </c>
@@ -493,8 +505,9 @@
       <c r="C6" s="5">
         <v>29</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="D6" s="5"/>
+    </row>
+    <row r="7" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>3002105</v>
       </c>
@@ -504,8 +517,9 @@
       <c r="C7" s="5">
         <v>29</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="D7" s="5"/>
+    </row>
+    <row r="8" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>3002106</v>
       </c>
@@ -515,6 +529,7 @@
       <c r="C8" s="5">
         <v>29</v>
       </c>
+      <c r="D8" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>